<commit_message>
Published state of ETDataset on 23 November 2020
</commit_message>
<xml_diff>
--- a/nodes_source_analyses/energy/energy/energy_production_synthetic_kerosene.xlsx
+++ b/nodes_source_analyses/energy/energy/energy_production_synthetic_kerosene.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10913"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11108"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michieldenhaan/Projects/etdataset/nodes_source_analyses/energy/energy/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marliekeverweij/Projects/etdataset/nodes_source_analyses/energy/energy/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CF45E61-477A-9F40-BAE0-3AC01A2E19BB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D214F8BF-5FBF-894A-9D03-83E051AE3EAC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="27180" tabRatio="762" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="27060" tabRatio="762" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover sheet" sheetId="14" r:id="rId1"/>
@@ -43,7 +43,7 @@
     <definedName name="Wp_to_kWp">#REF!</definedName>
     <definedName name="WP_to_MWp">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" calcOnSave="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="278">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="280">
   <si>
     <t>Source</t>
   </si>
@@ -881,9 +881,6 @@
     <t xml:space="preserve">Investment </t>
   </si>
   <si>
-    <t>Hoeveel CO nodig voor 10 PJ olieproducten?</t>
-  </si>
-  <si>
     <t>PJ/year</t>
   </si>
   <si>
@@ -902,9 +899,6 @@
     <t>The carbon conversion efficiency to fuels is 88%, the remaining 12% is converted into fuel that is not a FT fuel output (e.g. ethane/methane) and is used as purge gas and burned with air/oxygen to produce CO2 in a flue gas.</t>
   </si>
   <si>
-    <t>kg/year</t>
-  </si>
-  <si>
     <t>ton/year</t>
   </si>
   <si>
@@ -957,6 +951,18 @@
   </si>
   <si>
     <t>energy_production_synthetic_kerosene</t>
+  </si>
+  <si>
+    <t>Hoeveel CO nodig voor 1 PJ olieproducten?</t>
+  </si>
+  <si>
+    <t>kg</t>
+  </si>
+  <si>
+    <t>ton</t>
+  </si>
+  <si>
+    <t>AANNAME: GEEN VERLIEZEN</t>
   </si>
 </sst>
 </file>
@@ -970,7 +976,7 @@
     <numFmt numFmtId="167" formatCode="0.00000"/>
     <numFmt numFmtId="168" formatCode="[$-413]mmm\-yy;@"/>
   </numFmts>
-  <fonts count="43">
+  <fonts count="44">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1267,6 +1273,13 @@
     <font>
       <b/>
       <sz val="14"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -2185,7 +2198,7 @@
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="225">
+  <cellXfs count="226">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="27" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="28" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -2478,6 +2491,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="1" fontId="21" fillId="2" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="42" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="43" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="34" fillId="12" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -3195,6 +3209,50 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>733391</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>76201</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>317499</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3E6306CD-B07D-1940-A9DA-055D75284AE8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7692991" y="1143001"/>
+          <a:ext cx="8817008" cy="11163299"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -3703,12 +3761,12 @@
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="3.5" style="30" customWidth="1"/>
-    <col min="2" max="2" width="11.5" style="21" customWidth="1"/>
-    <col min="3" max="3" width="38.5" style="21" customWidth="1"/>
-    <col min="4" max="16384" width="10.83203125" style="21"/>
+    <col min="1" max="1" width="3.42578125" style="30" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" style="21" customWidth="1"/>
+    <col min="3" max="3" width="38.42578125" style="21" customWidth="1"/>
+    <col min="4" max="16384" width="10.85546875" style="21"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="28" customFormat="1">
@@ -3734,7 +3792,7 @@
         <v>10</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -3882,57 +3940,57 @@
   </sheetPr>
   <dimension ref="A1:K44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="2" width="3.5" style="34" customWidth="1"/>
-    <col min="3" max="3" width="51.5" style="34" customWidth="1"/>
-    <col min="4" max="5" width="14.6640625" style="34" customWidth="1"/>
-    <col min="6" max="6" width="4.5" style="34" customWidth="1"/>
-    <col min="7" max="7" width="49.5" style="34" customWidth="1"/>
-    <col min="8" max="8" width="20.83203125" style="34" customWidth="1"/>
-    <col min="9" max="9" width="42.5" style="34" customWidth="1"/>
-    <col min="10" max="10" width="5.5" style="34" customWidth="1"/>
-    <col min="11" max="16384" width="10.83203125" style="34"/>
+    <col min="1" max="2" width="3.42578125" style="34" customWidth="1"/>
+    <col min="3" max="3" width="51.42578125" style="34" customWidth="1"/>
+    <col min="4" max="5" width="14.7109375" style="34" customWidth="1"/>
+    <col min="6" max="6" width="4.42578125" style="34" customWidth="1"/>
+    <col min="7" max="7" width="49.42578125" style="34" customWidth="1"/>
+    <col min="8" max="8" width="20.85546875" style="34" customWidth="1"/>
+    <col min="9" max="9" width="42.42578125" style="34" customWidth="1"/>
+    <col min="10" max="10" width="5.42578125" style="34" customWidth="1"/>
+    <col min="11" max="16384" width="10.85546875" style="34"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
       <c r="D1" s="35"/>
     </row>
     <row r="2" spans="1:11">
-      <c r="B2" s="216" t="s">
+      <c r="B2" s="217" t="s">
         <v>72</v>
       </c>
-      <c r="C2" s="217"/>
-      <c r="D2" s="217"/>
-      <c r="E2" s="218"/>
+      <c r="C2" s="218"/>
+      <c r="D2" s="218"/>
+      <c r="E2" s="219"/>
       <c r="F2" s="35"/>
       <c r="G2" s="35"/>
     </row>
     <row r="3" spans="1:11">
-      <c r="B3" s="219"/>
-      <c r="C3" s="220"/>
-      <c r="D3" s="220"/>
-      <c r="E3" s="221"/>
+      <c r="B3" s="220"/>
+      <c r="C3" s="221"/>
+      <c r="D3" s="221"/>
+      <c r="E3" s="222"/>
       <c r="F3" s="35"/>
       <c r="G3" s="35"/>
     </row>
     <row r="4" spans="1:11">
-      <c r="B4" s="219"/>
-      <c r="C4" s="220"/>
-      <c r="D4" s="220"/>
-      <c r="E4" s="221"/>
+      <c r="B4" s="220"/>
+      <c r="C4" s="221"/>
+      <c r="D4" s="221"/>
+      <c r="E4" s="222"/>
       <c r="F4" s="35"/>
       <c r="G4" s="35"/>
     </row>
     <row r="5" spans="1:11">
-      <c r="B5" s="222"/>
-      <c r="C5" s="223"/>
-      <c r="D5" s="223"/>
-      <c r="E5" s="224"/>
+      <c r="B5" s="223"/>
+      <c r="C5" s="224"/>
+      <c r="D5" s="224"/>
+      <c r="E5" s="225"/>
       <c r="F5" s="35"/>
       <c r="G5" s="35"/>
     </row>
@@ -4027,7 +4085,7 @@
       <c r="D13" s="138"/>
       <c r="E13" s="146">
         <f>'Research data'!H8</f>
-        <v>7.6406122221098702E-2</v>
+        <v>0.44871705553657187</v>
       </c>
       <c r="F13" s="137"/>
       <c r="G13" s="147"/>
@@ -4045,7 +4103,7 @@
       </c>
       <c r="E14" s="146">
         <f>'Research data'!H9</f>
-        <v>0.92359387777890134</v>
+        <v>0.55128294446342818</v>
       </c>
       <c r="F14" s="38"/>
       <c r="G14" s="92"/>
@@ -4065,7 +4123,7 @@
       </c>
       <c r="E15" s="146">
         <f>'Research data'!H10</f>
-        <v>0.76583932824392909</v>
+        <v>0.75</v>
       </c>
       <c r="F15" s="92"/>
       <c r="G15" s="127"/>
@@ -4084,7 +4142,7 @@
       </c>
       <c r="E16" s="146">
         <f>'Research data'!H12</f>
-        <v>0.23416067175607091</v>
+        <v>0.25</v>
       </c>
       <c r="F16" s="92"/>
       <c r="G16" s="92"/>
@@ -4522,27 +4580,27 @@
   <dimension ref="A2:P28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="3.5" style="41" customWidth="1"/>
+    <col min="1" max="1" width="3.42578125" style="41" customWidth="1"/>
     <col min="2" max="2" width="3" style="41" customWidth="1"/>
     <col min="3" max="3" width="61" style="41" customWidth="1"/>
-    <col min="4" max="4" width="16.5" style="41" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="13.83203125" style="41" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="16.42578125" style="41" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" style="41" hidden="1" customWidth="1"/>
     <col min="6" max="6" width="10" style="41" customWidth="1"/>
     <col min="7" max="7" width="3" style="41" customWidth="1"/>
-    <col min="8" max="8" width="14.83203125" style="41" customWidth="1"/>
-    <col min="9" max="9" width="2.5" style="41" customWidth="1"/>
-    <col min="10" max="10" width="13.5" style="41" customWidth="1"/>
-    <col min="11" max="12" width="2.5" style="41" customWidth="1"/>
-    <col min="13" max="13" width="23.5" style="41" customWidth="1"/>
+    <col min="8" max="8" width="14.85546875" style="41" customWidth="1"/>
+    <col min="9" max="9" width="2.42578125" style="41" customWidth="1"/>
+    <col min="10" max="10" width="13.42578125" style="41" customWidth="1"/>
+    <col min="11" max="12" width="2.42578125" style="41" customWidth="1"/>
+    <col min="13" max="13" width="23.42578125" style="41" customWidth="1"/>
     <col min="14" max="14" width="11" style="41" customWidth="1"/>
-    <col min="15" max="15" width="2.5" style="41" customWidth="1"/>
-    <col min="16" max="16" width="22.5" style="41" customWidth="1"/>
-    <col min="17" max="16384" width="10.83203125" style="41"/>
+    <col min="15" max="15" width="2.42578125" style="41" customWidth="1"/>
+    <col min="16" max="16" width="22.42578125" style="41" customWidth="1"/>
+    <col min="17" max="16384" width="10.85546875" style="41"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:16" ht="17" thickBot="1"/>
@@ -4579,7 +4637,7 @@
       </c>
       <c r="I4" s="84"/>
       <c r="J4" s="84" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="K4" s="84"/>
       <c r="L4" s="84"/>
@@ -4655,11 +4713,11 @@
       <c r="G8" s="92"/>
       <c r="H8" s="128">
         <f t="shared" ref="H8:H12" si="0">J8</f>
-        <v>7.6406122221098702E-2</v>
+        <v>0.44871705553657187</v>
       </c>
       <c r="J8" s="155">
         <f>Notes!F14</f>
-        <v>7.6406122221098702E-2</v>
+        <v>0.44871705553657187</v>
       </c>
       <c r="K8" s="25"/>
     </row>
@@ -4679,11 +4737,11 @@
       <c r="G9" s="127"/>
       <c r="H9" s="128">
         <f t="shared" si="0"/>
-        <v>0.92359387777890134</v>
+        <v>0.55128294446342818</v>
       </c>
       <c r="J9" s="155">
         <f>Notes!F13</f>
-        <v>0.92359387777890134</v>
+        <v>0.55128294446342818</v>
       </c>
       <c r="K9" s="35"/>
     </row>
@@ -4703,11 +4761,11 @@
       <c r="G10" s="92"/>
       <c r="H10" s="128">
         <f>J10+J11</f>
-        <v>0.76583932824392909</v>
+        <v>0.75</v>
       </c>
       <c r="J10" s="155">
-        <f>Notes!E101</f>
-        <v>0.46801292281573448</v>
+        <f>Notes!D36</f>
+        <v>0.5</v>
       </c>
       <c r="K10" s="35"/>
     </row>
@@ -4726,8 +4784,8 @@
       <c r="G11" s="92"/>
       <c r="H11" s="128"/>
       <c r="J11" s="155">
-        <f>Notes!E102</f>
-        <v>0.29782640542819461</v>
+        <f>Notes!D37</f>
+        <v>0.25</v>
       </c>
       <c r="M11" s="167" t="s">
         <v>131</v>
@@ -4746,11 +4804,11 @@
       <c r="G12" s="92"/>
       <c r="H12" s="128">
         <f t="shared" si="0"/>
-        <v>0.23416067175607091</v>
+        <v>0.25</v>
       </c>
       <c r="J12" s="155">
-        <f>Notes!E103</f>
-        <v>0.23416067175607091</v>
+        <f>Notes!D38</f>
+        <v>0.25</v>
       </c>
     </row>
     <row r="13" spans="1:16" ht="17" thickBot="1">
@@ -5111,19 +5169,19 @@
       <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="33.1640625" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="33.140625" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="3.5" style="52" customWidth="1"/>
-    <col min="2" max="2" width="16.33203125" style="52" customWidth="1"/>
-    <col min="3" max="3" width="24.5" style="52" customWidth="1"/>
-    <col min="4" max="4" width="32.83203125" style="52" customWidth="1"/>
-    <col min="5" max="5" width="6.1640625" style="52" customWidth="1"/>
-    <col min="6" max="6" width="16.33203125" style="52" customWidth="1"/>
+    <col min="1" max="1" width="3.42578125" style="52" customWidth="1"/>
+    <col min="2" max="2" width="16.28515625" style="52" customWidth="1"/>
+    <col min="3" max="3" width="24.42578125" style="52" customWidth="1"/>
+    <col min="4" max="4" width="32.85546875" style="52" customWidth="1"/>
+    <col min="5" max="5" width="6.140625" style="52" customWidth="1"/>
+    <col min="6" max="6" width="16.28515625" style="52" customWidth="1"/>
     <col min="7" max="7" width="78" style="52" customWidth="1"/>
-    <col min="8" max="8" width="12.5" style="56" customWidth="1"/>
-    <col min="9" max="9" width="31.5" style="56" customWidth="1"/>
-    <col min="10" max="10" width="98.5" style="52" customWidth="1"/>
-    <col min="11" max="16384" width="33.1640625" style="52"/>
+    <col min="8" max="8" width="12.42578125" style="56" customWidth="1"/>
+    <col min="9" max="9" width="31.42578125" style="56" customWidth="1"/>
+    <col min="10" max="10" width="98.42578125" style="52" customWidth="1"/>
+    <col min="11" max="16384" width="33.140625" style="52"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:10" ht="17" thickBot="1"/>
@@ -5205,22 +5263,22 @@
         <v>228</v>
       </c>
       <c r="C7" s="213" t="s">
+        <v>266</v>
+      </c>
+      <c r="D7" s="213" t="s">
+        <v>269</v>
+      </c>
+      <c r="E7" s="213" t="s">
         <v>268</v>
-      </c>
-      <c r="D7" s="213" t="s">
-        <v>271</v>
-      </c>
-      <c r="E7" s="213" t="s">
-        <v>270</v>
       </c>
       <c r="F7" s="52">
         <v>2020</v>
       </c>
       <c r="G7" s="52" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="I7" s="56" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="8" spans="2:10">
@@ -5378,7 +5436,7 @@
     </row>
     <row r="19" spans="2:7">
       <c r="F19" s="213" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
     </row>
   </sheetData>
@@ -5395,22 +5453,22 @@
   </sheetPr>
   <dimension ref="A1:P294"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E48" sqref="E48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="2" width="3.5" style="60" customWidth="1"/>
-    <col min="3" max="3" width="18.5" style="60" customWidth="1"/>
+    <col min="1" max="2" width="3.42578125" style="60" customWidth="1"/>
+    <col min="3" max="3" width="18.42578125" style="60" customWidth="1"/>
     <col min="4" max="4" width="19" style="60" customWidth="1"/>
     <col min="5" max="5" width="17" style="60" customWidth="1"/>
-    <col min="6" max="6" width="6.1640625" style="60" customWidth="1"/>
-    <col min="7" max="13" width="10.83203125" style="60"/>
-    <col min="14" max="14" width="15.6640625" style="60" customWidth="1"/>
-    <col min="15" max="15" width="10.83203125" style="60"/>
-    <col min="16" max="16" width="12.1640625" style="60" customWidth="1"/>
-    <col min="17" max="16384" width="10.83203125" style="60"/>
+    <col min="6" max="6" width="6.140625" style="60" customWidth="1"/>
+    <col min="7" max="13" width="10.85546875" style="60"/>
+    <col min="14" max="14" width="15.7109375" style="60" customWidth="1"/>
+    <col min="15" max="15" width="10.85546875" style="60"/>
+    <col min="16" max="16" width="12.140625" style="60" customWidth="1"/>
+    <col min="17" max="16384" width="10.85546875" style="60"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="17" thickBot="1"/>
@@ -5471,7 +5529,7 @@
       <c r="A5" s="64"/>
       <c r="B5" s="149"/>
       <c r="C5" s="150" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D5" s="150"/>
       <c r="E5" s="150"/>
@@ -5521,7 +5579,7 @@
         <v>8322</v>
       </c>
       <c r="E7" s="67" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="F7" s="210" t="s">
         <v>228</v>
@@ -5602,11 +5660,11 @@
       <c r="B11" s="149"/>
       <c r="C11" s="67"/>
       <c r="D11" s="163">
-        <f>(D67*1000)/(SUM(E101,E102)*1000000000)</f>
-        <v>1.0870437202667023</v>
+        <f>(D67*1000)/(SUM(D36:D37)*1000000000)</f>
+        <v>0.11093668236525381</v>
       </c>
       <c r="E11" s="67" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="F11" s="150"/>
       <c r="G11" s="150"/>
@@ -5622,7 +5680,7 @@
       <c r="A12" s="64"/>
       <c r="B12" s="159"/>
       <c r="C12" s="150" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="D12" s="158"/>
       <c r="F12" s="67" t="s">
@@ -5645,14 +5703,14 @@
       </c>
       <c r="D13" s="158">
         <f>D66+D40</f>
-        <v>11.000040367795471</v>
+        <v>1.1180040367795472</v>
       </c>
       <c r="E13" s="67" t="s">
         <v>230</v>
       </c>
       <c r="F13" s="67">
         <f>D13/D15</f>
-        <v>0.92359387777890134</v>
+        <v>0.55128294446342818</v>
       </c>
       <c r="G13" s="150"/>
       <c r="H13" s="67"/>
@@ -5678,7 +5736,7 @@
       </c>
       <c r="F14" s="67">
         <f>D14/D15</f>
-        <v>7.6406122221098702E-2</v>
+        <v>0.44871705553657187</v>
       </c>
       <c r="G14" s="150"/>
       <c r="H14" s="67"/>
@@ -5693,11 +5751,11 @@
       <c r="A15" s="64"/>
       <c r="B15" s="149"/>
       <c r="C15" s="67" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="D15" s="158">
         <f>SUM(D13:D14)</f>
-        <v>11.910040367795471</v>
+        <v>2.0280040367795471</v>
       </c>
       <c r="E15" s="67"/>
       <c r="F15" s="67"/>
@@ -5762,7 +5820,7 @@
       <c r="A19" s="64"/>
       <c r="B19" s="149"/>
       <c r="C19" s="150" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="D19" s="150"/>
       <c r="E19" s="150"/>
@@ -5805,7 +5863,7 @@
         <v>10</v>
       </c>
       <c r="E21" s="67" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="F21" s="60" t="s">
         <v>232</v>
@@ -5827,7 +5885,7 @@
         <v>2777777.7777777775</v>
       </c>
       <c r="E22" s="67" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="H22" s="67"/>
       <c r="I22" s="67"/>
@@ -5953,7 +6011,7 @@
         <v>0.88</v>
       </c>
       <c r="E28" s="67" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="F28" s="67"/>
       <c r="G28" s="150"/>
@@ -6289,15 +6347,15 @@
       <c r="A45" s="64"/>
       <c r="B45" s="149"/>
       <c r="C45" s="67" t="s">
-        <v>252</v>
+        <v>276</v>
       </c>
       <c r="D45" s="67"/>
       <c r="E45" s="67">
-        <f>D21*D42</f>
-        <v>5.3000000000000007</v>
+        <f>D42</f>
+        <v>0.53</v>
       </c>
       <c r="F45" s="67" t="s">
-        <v>253</v>
+        <v>230</v>
       </c>
       <c r="G45" s="150"/>
       <c r="H45" s="67"/>
@@ -6317,7 +6375,7 @@
         <v>1000</v>
       </c>
       <c r="F46" s="67" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="G46" s="150"/>
       <c r="H46" s="67"/>
@@ -6335,10 +6393,10 @@
       <c r="D47" s="67"/>
       <c r="E47" s="67">
         <f>E45*1000000000/E91</f>
-        <v>529470529.47052956</v>
+        <v>52947052.947052948</v>
       </c>
       <c r="F47" s="67" t="s">
-        <v>259</v>
+        <v>277</v>
       </c>
       <c r="G47" s="150"/>
       <c r="H47" s="67"/>
@@ -6356,10 +6414,10 @@
       <c r="D48" s="67"/>
       <c r="E48" s="67">
         <f>E47/E46</f>
-        <v>529470.52947052952</v>
+        <v>52947.052947052951</v>
       </c>
       <c r="F48" s="67" t="s">
-        <v>260</v>
+        <v>278</v>
       </c>
       <c r="G48" s="150"/>
       <c r="H48" s="67"/>
@@ -6493,14 +6551,14 @@
       <c r="A55" s="64"/>
       <c r="B55" s="149"/>
       <c r="C55" s="67" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D55" s="67">
-        <f>E45</f>
+        <f>E45*D21</f>
         <v>5.3000000000000007</v>
       </c>
       <c r="E55" s="67" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="F55" s="67"/>
       <c r="G55" s="150"/>
@@ -6521,7 +6579,7 @@
         <v>1472222.2222222222</v>
       </c>
       <c r="E56" s="67" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="F56" s="67"/>
       <c r="G56" s="150"/>
@@ -6601,10 +6659,11 @@
       <c r="B60" s="149"/>
       <c r="C60" s="67"/>
       <c r="D60" s="67">
-        <v>0.63600000000000001</v>
+        <f>E157/E158</f>
+        <v>0.63636363636363635</v>
       </c>
       <c r="E60" s="67" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="F60" s="67"/>
       <c r="G60" s="150"/>
@@ -6657,7 +6716,8 @@
         <v>85</v>
       </c>
       <c r="D63" s="67">
-        <v>5.3</v>
+        <f>E45</f>
+        <v>0.53</v>
       </c>
       <c r="E63" s="67" t="s">
         <v>230</v>
@@ -6693,14 +6753,14 @@
       <c r="A65" s="64"/>
       <c r="B65" s="149"/>
       <c r="C65" s="67" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="D65" s="158">
         <f>E48*E177</f>
-        <v>3050011213.2765198</v>
+        <v>305001121.32765198</v>
       </c>
       <c r="E65" s="60" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="F65" s="67"/>
       <c r="G65" s="150"/>
@@ -6718,7 +6778,7 @@
       <c r="C66" s="67"/>
       <c r="D66" s="158">
         <f>D65*3.6/1000000000</f>
-        <v>10.980040367795471</v>
+        <v>1.0980040367795472</v>
       </c>
       <c r="E66" s="60" t="s">
         <v>230</v>
@@ -6740,20 +6800,23 @@
       </c>
       <c r="D67" s="60">
         <f>E48/D60</f>
-        <v>832500.83250083262</v>
+        <v>83202.51177394035</v>
       </c>
       <c r="E67" s="60" t="s">
-        <v>260</v>
+        <v>258</v>
+      </c>
+      <c r="F67" s="216" t="s">
+        <v>279</v>
       </c>
     </row>
     <row r="68" spans="1:14">
       <c r="B68" s="185"/>
       <c r="D68" s="60">
         <f>D67/1000000</f>
-        <v>0.83250083250083262</v>
+        <v>8.3202511773940349E-2</v>
       </c>
       <c r="E68" s="60" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
     </row>
     <row r="69" spans="1:14" ht="17" customHeight="1">

</xml_diff>